<commit_message>
Color coded column headers
</commit_message>
<xml_diff>
--- a/files/data (csv and rda)/data.NHS.2012_2019.xlsx
+++ b/files/data (csv and rda)/data.NHS.2012_2019.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Owner\Dropbox\work\QI\Intangibles\Innovation\_NHS SMHI study\Boyle study\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{2AF7E321-1B3A-4D29-A77F-DD441EBF02FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD5E2E6B-CF7F-4485-863F-7DE5AB249854}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25920" yWindow="420" windowWidth="20970" windowHeight="14220"/>
+    <workbookView xWindow="25920" yWindow="420" windowWidth="20970" windowHeight="14220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data.NHS.2012_2019" sheetId="1" r:id="rId1"/>
@@ -1054,7 +1054,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1191,7 +1191,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="36">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1389,6 +1389,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -1550,12 +1556,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1910,11 +1917,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U1085"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S5" sqref="S5"/>
+      <selection activeCell="Q7" sqref="Q7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1974,7 +1981,7 @@
       <c r="R1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="S1" s="5" t="s">
         <v>18</v>
       </c>
       <c r="T1" t="s">

</xml_diff>